<commit_message>
brought cost last and centered the values
</commit_message>
<xml_diff>
--- a/output/status_project_report.xlsx
+++ b/output/status_project_report.xlsx
@@ -120,8 +120,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -501,12 +505,12 @@
     <col width="11" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="9" customWidth="1" min="8" max="8"/>
-    <col width="10" customWidth="1" min="9" max="9"/>
-    <col width="18" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
-    <col width="21" customWidth="1" min="12" max="12"/>
+    <col width="9" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="18" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
     <col hidden="1" width="13" customWidth="1" min="13" max="13"/>
     <col hidden="1" width="13" customWidth="1" min="14" max="14"/>
     <col hidden="1" width="13" customWidth="1" min="15" max="15"/>
@@ -558,32 +562,32 @@
       </c>
       <c r="G2" s="3" t="inlineStr">
         <is>
+          <t>On Hold</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>Released</t>
+        </is>
+      </c>
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>Vehicle Released</t>
+        </is>
+      </c>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>Workshop Completed</t>
+        </is>
+      </c>
+      <c r="K2" s="3" t="inlineStr">
+        <is>
+          <t>Workshop Checked In</t>
+        </is>
+      </c>
+      <c r="L2" s="3" t="inlineStr">
+        <is>
           <t>Material cost</t>
-        </is>
-      </c>
-      <c r="H2" s="3" t="inlineStr">
-        <is>
-          <t>On Hold</t>
-        </is>
-      </c>
-      <c r="I2" s="3" t="inlineStr">
-        <is>
-          <t>Released</t>
-        </is>
-      </c>
-      <c r="J2" s="3" t="inlineStr">
-        <is>
-          <t>Vehicle Released</t>
-        </is>
-      </c>
-      <c r="K2" s="3" t="inlineStr">
-        <is>
-          <t>Workshop Completed</t>
-        </is>
-      </c>
-      <c r="L2" s="3" t="inlineStr">
-        <is>
-          <t>Workshop Checked In</t>
         </is>
       </c>
     </row>
@@ -611,7 +615,7 @@
         <v>32</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>44.66468055607378</v>
+        <v>0</v>
       </c>
       <c r="H3" s="5" t="n">
         <v>0</v>
@@ -623,10 +627,10 @@
         <v>0</v>
       </c>
       <c r="K3" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L3" s="5" t="n">
-        <v>2</v>
+        <v>44.67</v>
       </c>
     </row>
     <row r="4">
@@ -877,7 +881,7 @@
         <v>43</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>44.66468055607378</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6" t="n">
         <v>0</v>
@@ -889,10 +893,10 @@
         <v>0</v>
       </c>
       <c r="K10" s="6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10" s="6" t="n">
-        <v>2</v>
+        <v>44.67</v>
       </c>
     </row>
     <row r="11">
@@ -919,22 +923,22 @@
         <v>5</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>137.1471533741143</v>
+        <v>0</v>
       </c>
       <c r="H11" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J11" s="5" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K11" s="5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L11" s="5" t="n">
-        <v>3</v>
+        <v>137.15</v>
       </c>
     </row>
     <row r="12">
@@ -957,22 +961,22 @@
         <v>0</v>
       </c>
       <c r="G12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="5" t="n">
         <v>189.4</v>
-      </c>
-      <c r="H12" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" s="5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -995,7 +999,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>100.525</v>
+        <v>0</v>
       </c>
       <c r="H13" s="5" t="n">
         <v>0</v>
@@ -1007,10 +1011,10 @@
         <v>0</v>
       </c>
       <c r="K13" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" s="5" t="n">
-        <v>1</v>
+        <v>100.53</v>
       </c>
     </row>
     <row r="14">
@@ -1033,22 +1037,22 @@
         <v>2</v>
       </c>
       <c r="G14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K14" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="L14" s="5" t="n">
         <v>49.25</v>
-      </c>
-      <c r="H14" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K14" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="L14" s="5" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="15">
@@ -1080,10 +1084,10 @@
         <v>0</v>
       </c>
       <c r="J15" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K15" s="5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L15" s="5" t="n">
         <v>0</v>
@@ -1109,13 +1113,13 @@
         <v>0</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>71.85003539998917</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="5" t="n">
         <v>1</v>
@@ -1124,7 +1128,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="5" t="n">
-        <v>1</v>
+        <v>71.84999999999999</v>
       </c>
     </row>
     <row r="17">
@@ -1147,22 +1151,22 @@
         <v>10</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>192.3000852523497</v>
+        <v>0</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J17" s="5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K17" s="5" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L17" s="5" t="n">
-        <v>4</v>
+        <v>192.3</v>
       </c>
     </row>
     <row r="18">
@@ -1185,22 +1189,22 @@
         <v>2</v>
       </c>
       <c r="G18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="I18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="5" t="n">
         <v>93</v>
-      </c>
-      <c r="H18" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="J18" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" s="5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1223,7 +1227,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>4.140182142709672</v>
+        <v>0</v>
       </c>
       <c r="H19" s="5" t="n">
         <v>0</v>
@@ -1232,13 +1236,13 @@
         <v>0</v>
       </c>
       <c r="J19" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="5" t="n">
-        <v>0</v>
+        <v>4.140000000000001</v>
       </c>
     </row>
     <row r="20">
@@ -1261,22 +1265,22 @@
         <v>0</v>
       </c>
       <c r="G20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="5" t="n">
         <v>0.82</v>
-      </c>
-      <c r="H20" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" s="5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1299,22 +1303,22 @@
         <v>24</v>
       </c>
       <c r="G21" s="6" t="n">
-        <v>838.4324561691629</v>
+        <v>0</v>
       </c>
       <c r="H21" s="6" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I21" s="6" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J21" s="6" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="K21" s="6" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="L21" s="6" t="n">
-        <v>16</v>
+        <v>838.4400000000001</v>
       </c>
     </row>
     <row r="22">
@@ -1350,10 +1354,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K22" s="5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L22" s="5" t="n">
         <v>0</v>
@@ -1379,22 +1383,22 @@
         <v>0</v>
       </c>
       <c r="G23" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K23" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="5" t="n">
         <v>133</v>
-      </c>
-      <c r="H23" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J23" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="L23" s="5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1423,10 +1427,10 @@
         <v>0</v>
       </c>
       <c r="I24" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24" s="5" t="n">
         <v>0</v>
@@ -1455,22 +1459,22 @@
         <v>0</v>
       </c>
       <c r="G25" s="5" t="n">
-        <v>355.3744760075709</v>
+        <v>0</v>
       </c>
       <c r="H25" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I25" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="5" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="K25" s="5" t="n">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="L25" s="5" t="n">
-        <v>3</v>
+        <v>355.3699999999999</v>
       </c>
     </row>
     <row r="26">
@@ -1493,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="5" t="n">
-        <v>90.0512065254678</v>
+        <v>0</v>
       </c>
       <c r="H26" s="5" t="n">
         <v>0</v>
@@ -1502,13 +1506,13 @@
         <v>0</v>
       </c>
       <c r="J26" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K26" s="5" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L26" s="5" t="n">
-        <v>1</v>
+        <v>90.05</v>
       </c>
     </row>
     <row r="27">
@@ -1543,10 +1547,10 @@
         <v>0</v>
       </c>
       <c r="K27" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L27" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1578,10 +1582,10 @@
         <v>0</v>
       </c>
       <c r="J28" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" s="5" t="n">
         <v>0</v>
@@ -1619,10 +1623,10 @@
         <v>0</v>
       </c>
       <c r="K29" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L29" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1645,22 +1649,22 @@
         <v>0</v>
       </c>
       <c r="G30" s="5" t="n">
-        <v>312.7499990286201</v>
+        <v>1</v>
       </c>
       <c r="H30" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J30" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K30" s="5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L30" s="5" t="n">
-        <v>0</v>
+        <v>312.75</v>
       </c>
     </row>
     <row r="31">
@@ -1683,7 +1687,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="5" t="n">
-        <v>767.1302059046885</v>
+        <v>0</v>
       </c>
       <c r="H31" s="5" t="n">
         <v>0</v>
@@ -1698,7 +1702,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="5" t="n">
-        <v>0</v>
+        <v>767.1299999999999</v>
       </c>
     </row>
     <row r="32">
@@ -1721,22 +1725,22 @@
         <v>0</v>
       </c>
       <c r="G32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" s="5" t="n">
         <v>12</v>
-      </c>
-      <c r="H32" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I32" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K32" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" s="5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1759,22 +1763,22 @@
         <v>0</v>
       </c>
       <c r="G33" s="6" t="n">
-        <v>1670.305887466347</v>
+        <v>1</v>
       </c>
       <c r="H33" s="6" t="n">
         <v>1</v>
       </c>
       <c r="I33" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J33" s="6" t="n">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="K33" s="6" t="n">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="L33" s="6" t="n">
-        <v>9</v>
+        <v>1670.299999999999</v>
       </c>
     </row>
     <row r="34">
@@ -1807,13 +1811,13 @@
         <v>0</v>
       </c>
       <c r="I34" s="5" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="J34" s="5" t="n">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="K34" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L34" s="5" t="n">
         <v>0</v>
@@ -1839,22 +1843,22 @@
         <v>0</v>
       </c>
       <c r="G35" s="5" t="n">
-        <v>178.5103138237088</v>
+        <v>0</v>
       </c>
       <c r="H35" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I35" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J35" s="5" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K35" s="5" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L35" s="5" t="n">
-        <v>0</v>
+        <v>178.51</v>
       </c>
     </row>
     <row r="36">
@@ -1886,10 +1890,10 @@
         <v>0</v>
       </c>
       <c r="J36" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L36" s="5" t="n">
         <v>0</v>
@@ -1915,22 +1919,22 @@
         <v>0</v>
       </c>
       <c r="G37" s="5" t="n">
-        <v>224.5</v>
+        <v>0</v>
       </c>
       <c r="H37" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J37" s="5" t="n">
         <v>2</v>
       </c>
       <c r="K37" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L37" s="5" t="n">
-        <v>0</v>
+        <v>224.5</v>
       </c>
     </row>
     <row r="38">
@@ -1953,22 +1957,22 @@
         <v>0</v>
       </c>
       <c r="G38" s="5" t="n">
-        <v>719.9001705046993</v>
+        <v>0</v>
       </c>
       <c r="H38" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" s="5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J38" s="5" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="K38" s="5" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="L38" s="5" t="n">
-        <v>3</v>
+        <v>719.9</v>
       </c>
     </row>
     <row r="39">
@@ -1991,22 +1995,22 @@
         <v>0</v>
       </c>
       <c r="G39" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="L39" s="5" t="n">
         <v>184.5</v>
-      </c>
-      <c r="H39" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I39" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J39" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K39" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L39" s="5" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -2035,10 +2039,10 @@
         <v>0</v>
       </c>
       <c r="I40" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40" s="5" t="n">
         <v>0</v>
@@ -2070,13 +2074,13 @@
         <v>0</v>
       </c>
       <c r="H41" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" s="5" t="n">
         <v>1</v>
       </c>
       <c r="J41" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K41" s="5" t="n">
         <v>0</v>
@@ -2105,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="5" t="n">
-        <v>83.3481652490736</v>
+        <v>0</v>
       </c>
       <c r="H42" s="5" t="n">
         <v>0</v>
@@ -2114,13 +2118,13 @@
         <v>0</v>
       </c>
       <c r="J42" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K42" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L42" s="5" t="n">
-        <v>0</v>
+        <v>83.34999999999999</v>
       </c>
     </row>
     <row r="43">
@@ -2143,22 +2147,22 @@
         <v>0</v>
       </c>
       <c r="G43" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" s="5" t="n">
         <v>20.7</v>
-      </c>
-      <c r="H43" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J43" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K43" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L43" s="5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -2181,7 +2185,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="5" t="n">
-        <v>0.825</v>
+        <v>0</v>
       </c>
       <c r="H44" s="5" t="n">
         <v>0</v>
@@ -2196,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="L44" s="5" t="n">
-        <v>0</v>
+        <v>0.8200000000000001</v>
       </c>
     </row>
     <row r="45">
@@ -2219,22 +2223,22 @@
         <v>0</v>
       </c>
       <c r="G45" s="6" t="n">
-        <v>1412.283649577482</v>
+        <v>0</v>
       </c>
       <c r="H45" s="6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I45" s="6" t="n">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="J45" s="6" t="n">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="K45" s="6" t="n">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="L45" s="6" t="n">
-        <v>5</v>
+        <v>1412.28</v>
       </c>
     </row>
     <row r="46">
@@ -2267,10 +2271,10 @@
         <v>0</v>
       </c>
       <c r="I46" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K46" s="5" t="n">
         <v>0</v>
@@ -2305,13 +2309,13 @@
         <v>0</v>
       </c>
       <c r="I47" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J47" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K47" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L47" s="5" t="n">
         <v>0</v>
@@ -2337,22 +2341,22 @@
         <v>0</v>
       </c>
       <c r="G48" s="5" t="n">
-        <v>213.0402912569807</v>
+        <v>0</v>
       </c>
       <c r="H48" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I48" s="5" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="J48" s="5" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="K48" s="5" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L48" s="5" t="n">
-        <v>1</v>
+        <v>213.04</v>
       </c>
     </row>
     <row r="49">
@@ -2375,22 +2379,22 @@
         <v>0</v>
       </c>
       <c r="G49" s="5" t="n">
-        <v>154.2499990286201</v>
+        <v>1</v>
       </c>
       <c r="H49" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" s="5" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J49" s="5" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K49" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L49" s="5" t="n">
-        <v>2</v>
+        <v>154.25</v>
       </c>
     </row>
     <row r="50">
@@ -2413,22 +2417,22 @@
         <v>0</v>
       </c>
       <c r="G50" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J50" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K50" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="L50" s="5" t="n">
         <v>0.52</v>
-      </c>
-      <c r="H50" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I50" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J50" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K50" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="L50" s="5" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="51">
@@ -2451,22 +2455,22 @@
         <v>0</v>
       </c>
       <c r="G51" s="5" t="n">
-        <v>115.6844054</v>
+        <v>0</v>
       </c>
       <c r="H51" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I51" s="5" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J51" s="5" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K51" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L51" s="5" t="n">
-        <v>1</v>
+        <v>115.68</v>
       </c>
     </row>
     <row r="52">
@@ -2489,22 +2493,22 @@
         <v>0</v>
       </c>
       <c r="G52" s="5" t="n">
-        <v>100.2499990286201</v>
+        <v>0</v>
       </c>
       <c r="H52" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I52" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K52" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L52" s="5" t="n">
-        <v>0</v>
+        <v>100.25</v>
       </c>
     </row>
     <row r="53">
@@ -2527,22 +2531,22 @@
         <v>0</v>
       </c>
       <c r="G53" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J53" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L53" s="5" t="n">
         <v>28</v>
-      </c>
-      <c r="H53" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I53" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J53" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K53" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L53" s="5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -2571,10 +2575,10 @@
         <v>0</v>
       </c>
       <c r="I54" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J54" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K54" s="5" t="n">
         <v>0</v>
@@ -2603,22 +2607,22 @@
         <v>0</v>
       </c>
       <c r="G55" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J55" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K55" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L55" s="5" t="n">
         <v>85.09</v>
-      </c>
-      <c r="H55" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I55" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J55" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K55" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L55" s="5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -2653,10 +2657,10 @@
         <v>0</v>
       </c>
       <c r="K56" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L56" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -2679,22 +2683,22 @@
         <v>0</v>
       </c>
       <c r="G57" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K57" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L57" s="5" t="n">
         <v>0.52</v>
-      </c>
-      <c r="H57" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I57" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J57" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K57" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L57" s="5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -2717,22 +2721,22 @@
         <v>0</v>
       </c>
       <c r="G58" s="6" t="n">
-        <v>697.3546947142208</v>
+        <v>1</v>
       </c>
       <c r="H58" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I58" s="6" t="n">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="J58" s="6" t="n">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="K58" s="6" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="L58" s="6" t="n">
-        <v>7</v>
+        <v>697.3499999999999</v>
       </c>
     </row>
     <row r="59">
@@ -2765,10 +2769,10 @@
         <v>0</v>
       </c>
       <c r="I59" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J59" s="5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K59" s="5" t="n">
         <v>0</v>
@@ -2797,22 +2801,22 @@
         <v>0</v>
       </c>
       <c r="G60" s="5" t="n">
-        <v>585.0000605094154</v>
+        <v>0</v>
       </c>
       <c r="H60" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I60" s="5" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J60" s="5" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K60" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L60" s="5" t="n">
-        <v>3</v>
+        <v>584.9999999999998</v>
       </c>
     </row>
     <row r="61">
@@ -2835,22 +2839,22 @@
         <v>0</v>
       </c>
       <c r="G61" s="5" t="n">
-        <v>69.17003549993169</v>
+        <v>0</v>
       </c>
       <c r="H61" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" s="5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J61" s="5" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K61" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L61" s="5" t="n">
-        <v>2</v>
+        <v>69.17</v>
       </c>
     </row>
     <row r="62">
@@ -2879,10 +2883,10 @@
         <v>0</v>
       </c>
       <c r="I62" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J62" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K62" s="5" t="n">
         <v>0</v>
@@ -2917,10 +2921,10 @@
         <v>0</v>
       </c>
       <c r="I63" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J63" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K63" s="5" t="n">
         <v>0</v>
@@ -2949,22 +2953,22 @@
         <v>0</v>
       </c>
       <c r="G64" s="5" t="n">
-        <v>241.2494788654942</v>
+        <v>0</v>
       </c>
       <c r="H64" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I64" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J64" s="5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K64" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L64" s="5" t="n">
-        <v>1</v>
+        <v>241.25</v>
       </c>
     </row>
     <row r="65">
@@ -2987,22 +2991,22 @@
         <v>0</v>
       </c>
       <c r="G65" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J65" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K65" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="L65" s="5" t="n">
         <v>209</v>
-      </c>
-      <c r="H65" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I65" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J65" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="K65" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L65" s="5" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="66">
@@ -3037,10 +3041,10 @@
         <v>0</v>
       </c>
       <c r="K66" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L66" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -3063,22 +3067,22 @@
         <v>0</v>
       </c>
       <c r="G67" s="5" t="n">
-        <v>230.378</v>
+        <v>1</v>
       </c>
       <c r="H67" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J67" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K67" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L67" s="5" t="n">
-        <v>0</v>
+        <v>230.38</v>
       </c>
     </row>
     <row r="68">
@@ -3107,10 +3111,10 @@
         <v>0</v>
       </c>
       <c r="I68" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J68" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K68" s="5" t="n">
         <v>0</v>
@@ -3145,10 +3149,10 @@
         <v>0</v>
       </c>
       <c r="I69" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J69" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K69" s="5" t="n">
         <v>0</v>
@@ -3177,7 +3181,7 @@
         <v>0</v>
       </c>
       <c r="G70" s="5" t="n">
-        <v>0.825</v>
+        <v>0</v>
       </c>
       <c r="H70" s="5" t="n">
         <v>0</v>
@@ -3192,7 +3196,7 @@
         <v>0</v>
       </c>
       <c r="L70" s="5" t="n">
-        <v>0</v>
+        <v>0.8200000000000001</v>
       </c>
     </row>
     <row r="71">
@@ -3215,22 +3219,22 @@
         <v>0</v>
       </c>
       <c r="G71" s="6" t="n">
-        <v>1335.622574874842</v>
+        <v>1</v>
       </c>
       <c r="H71" s="6" t="n">
         <v>1</v>
       </c>
       <c r="I71" s="6" t="n">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="J71" s="6" t="n">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="K71" s="6" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L71" s="6" t="n">
-        <v>10</v>
+        <v>1335.62</v>
       </c>
     </row>
     <row r="72">
@@ -3257,22 +3261,22 @@
         <v>0</v>
       </c>
       <c r="G72" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="J72" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K72" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L72" s="5" t="n">
         <v>37.25</v>
-      </c>
-      <c r="H72" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I72" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J72" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="K72" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L72" s="5" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -3301,10 +3305,10 @@
         <v>0</v>
       </c>
       <c r="I73" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J73" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K73" s="5" t="n">
         <v>0</v>
@@ -3333,22 +3337,22 @@
         <v>0</v>
       </c>
       <c r="G74" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="J74" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K74" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L74" s="5" t="n">
         <v>96.08</v>
-      </c>
-      <c r="H74" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I74" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J74" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="K74" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L74" s="5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -3371,22 +3375,22 @@
         <v>0</v>
       </c>
       <c r="G75" s="5" t="n">
-        <v>122.1600852523497</v>
+        <v>0</v>
       </c>
       <c r="H75" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I75" s="5" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J75" s="5" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K75" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L75" s="5" t="n">
-        <v>2</v>
+        <v>122.16</v>
       </c>
     </row>
     <row r="76">
@@ -3415,10 +3419,10 @@
         <v>0</v>
       </c>
       <c r="I76" s="5" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J76" s="5" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K76" s="5" t="n">
         <v>0</v>
@@ -3459,10 +3463,10 @@
         <v>0</v>
       </c>
       <c r="K77" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L77" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -3491,10 +3495,10 @@
         <v>0</v>
       </c>
       <c r="I78" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J78" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K78" s="5" t="n">
         <v>0</v>
@@ -3523,22 +3527,22 @@
         <v>0</v>
       </c>
       <c r="G79" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K79" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L79" s="5" t="n">
         <v>45</v>
-      </c>
-      <c r="H79" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I79" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J79" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K79" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L79" s="5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -3561,22 +3565,22 @@
         <v>0</v>
       </c>
       <c r="G80" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K80" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L80" s="5" t="n">
         <v>7</v>
-      </c>
-      <c r="H80" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I80" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J80" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K80" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L80" s="5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -3599,7 +3603,7 @@
         <v>0</v>
       </c>
       <c r="G81" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81" s="5" t="n">
         <v>0</v>
@@ -3614,7 +3618,7 @@
         <v>0</v>
       </c>
       <c r="L81" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -3637,22 +3641,22 @@
         <v>0</v>
       </c>
       <c r="G82" s="6" t="n">
-        <v>308.4900852523497</v>
+        <v>0</v>
       </c>
       <c r="H82" s="6" t="n">
         <v>0</v>
       </c>
       <c r="I82" s="6" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J82" s="6" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="K82" s="6" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L82" s="6" t="n">
-        <v>4</v>
+        <v>308.49</v>
       </c>
     </row>
     <row r="83">
@@ -3685,10 +3689,10 @@
         <v>0</v>
       </c>
       <c r="I83" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J83" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K83" s="5" t="n">
         <v>0</v>
@@ -3723,10 +3727,10 @@
         <v>0</v>
       </c>
       <c r="I84" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J84" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K84" s="5" t="n">
         <v>0</v>
@@ -3755,22 +3759,22 @@
         <v>0</v>
       </c>
       <c r="G85" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="J85" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K85" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L85" s="5" t="n">
         <v>13</v>
-      </c>
-      <c r="H85" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I85" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J85" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="K85" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L85" s="5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -3799,10 +3803,10 @@
         <v>0</v>
       </c>
       <c r="I86" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J86" s="5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K86" s="5" t="n">
         <v>0</v>
@@ -3837,10 +3841,10 @@
         <v>0</v>
       </c>
       <c r="I87" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J87" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K87" s="5" t="n">
         <v>0</v>
@@ -3875,10 +3879,10 @@
         <v>0</v>
       </c>
       <c r="I88" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J88" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K88" s="5" t="n">
         <v>0</v>
@@ -3913,10 +3917,10 @@
         <v>0</v>
       </c>
       <c r="I89" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J89" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K89" s="5" t="n">
         <v>0</v>
@@ -3945,22 +3949,22 @@
         <v>0</v>
       </c>
       <c r="G90" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K90" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L90" s="5" t="n">
         <v>35</v>
-      </c>
-      <c r="H90" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I90" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J90" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K90" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L90" s="5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -3983,22 +3987,22 @@
         <v>0</v>
       </c>
       <c r="G91" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" s="6" t="n">
+        <v>31</v>
+      </c>
+      <c r="J91" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K91" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L91" s="6" t="n">
         <v>48</v>
-      </c>
-      <c r="H91" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I91" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J91" s="6" t="n">
-        <v>31</v>
-      </c>
-      <c r="K91" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L91" s="6" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="92" hidden="1"/>

</xml_diff>

<commit_message>
added month-wise status report
</commit_message>
<xml_diff>
--- a/output/status_project_report.xlsx
+++ b/output/status_project_report.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Project Status Report" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="day_wise_Status_Report" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="month_wise_Status_Report" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -55,7 +56,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -102,11 +103,53 @@
       <bottom style="thick"/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick"/>
+      <top/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick"/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -126,6 +169,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -511,15 +558,6 @@
     <col width="20" customWidth="1" min="10" max="10"/>
     <col width="21" customWidth="1" min="11" max="11"/>
     <col width="20" customWidth="1" min="12" max="12"/>
-    <col hidden="1" width="13" customWidth="1" min="13" max="13"/>
-    <col hidden="1" width="13" customWidth="1" min="14" max="14"/>
-    <col hidden="1" width="13" customWidth="1" min="15" max="15"/>
-    <col hidden="1" width="13" customWidth="1" min="16" max="16"/>
-    <col hidden="1" width="13" customWidth="1" min="17" max="17"/>
-    <col hidden="1" width="13" customWidth="1" min="18" max="18"/>
-    <col hidden="1" width="13" customWidth="1" min="19" max="19"/>
-    <col hidden="1" width="13" customWidth="1" min="20" max="20"/>
-    <col hidden="1" width="13" customWidth="1" min="21" max="21"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -528,6 +566,17 @@
           <t>Work Order Status Report</t>
         </is>
       </c>
+      <c r="B1" s="7" t="n"/>
+      <c r="C1" s="7" t="n"/>
+      <c r="D1" s="7" t="n"/>
+      <c r="E1" s="7" t="n"/>
+      <c r="F1" s="7" t="n"/>
+      <c r="G1" s="7" t="n"/>
+      <c r="H1" s="7" t="n"/>
+      <c r="I1" s="7" t="n"/>
+      <c r="J1" s="7" t="n"/>
+      <c r="K1" s="7" t="n"/>
+      <c r="L1" s="8" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -634,7 +683,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="n"/>
+      <c r="A4" s="9" t="n"/>
       <c r="B4" s="5" t="inlineStr">
         <is>
           <t>TC-ES</t>
@@ -672,7 +721,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="n"/>
+      <c r="A5" s="9" t="n"/>
       <c r="B5" s="5" t="inlineStr">
         <is>
           <t>TC-US Govt</t>
@@ -710,7 +759,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="n"/>
+      <c r="A6" s="9" t="n"/>
       <c r="B6" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -748,7 +797,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="n"/>
+      <c r="A7" s="9" t="n"/>
       <c r="B7" s="5" t="inlineStr">
         <is>
           <t>TC-KT</t>
@@ -786,7 +835,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="n"/>
+      <c r="A8" s="9" t="n"/>
       <c r="B8" s="5" t="inlineStr">
         <is>
           <t>TC-BLKLT</t>
@@ -824,7 +873,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="n"/>
+      <c r="A9" s="9" t="n"/>
       <c r="B9" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -862,7 +911,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="n"/>
+      <c r="A10" s="9" t="n"/>
       <c r="B10" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -900,7 +949,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="n"/>
+      <c r="A11" s="10" t="n"/>
       <c r="B11" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -980,7 +1029,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="n"/>
+      <c r="A13" s="9" t="n"/>
       <c r="B13" s="5" t="inlineStr">
         <is>
           <t>FS-PV</t>
@@ -1018,7 +1067,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="n"/>
+      <c r="A14" s="9" t="n"/>
       <c r="B14" s="5" t="inlineStr">
         <is>
           <t>TC-US Govt</t>
@@ -1056,7 +1105,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="n"/>
+      <c r="A15" s="9" t="n"/>
       <c r="B15" s="5" t="inlineStr">
         <is>
           <t>TC-ES</t>
@@ -1094,7 +1143,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="n"/>
+      <c r="A16" s="9" t="n"/>
       <c r="B16" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -1132,7 +1181,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="n"/>
+      <c r="A17" s="9" t="n"/>
       <c r="B17" s="5" t="inlineStr">
         <is>
           <t>TC-MHECRAN</t>
@@ -1170,7 +1219,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="n"/>
+      <c r="A18" s="9" t="n"/>
       <c r="B18" s="5" t="inlineStr">
         <is>
           <t>TC-TERMINL</t>
@@ -1208,7 +1257,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="n"/>
+      <c r="A19" s="9" t="n"/>
       <c r="B19" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -1246,7 +1295,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="n"/>
+      <c r="A20" s="9" t="n"/>
       <c r="B20" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -1284,7 +1333,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="n"/>
+      <c r="A21" s="9" t="n"/>
       <c r="B21" s="5" t="inlineStr">
         <is>
           <t>TC-BLKLT</t>
@@ -1322,7 +1371,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="n"/>
+      <c r="A22" s="10" t="n"/>
       <c r="B22" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -1402,7 +1451,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="n"/>
+      <c r="A24" s="9" t="n"/>
       <c r="B24" s="5" t="inlineStr">
         <is>
           <t>TC-KT</t>
@@ -1440,7 +1489,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="n"/>
+      <c r="A25" s="9" t="n"/>
       <c r="B25" s="5" t="inlineStr">
         <is>
           <t>FS-PV</t>
@@ -1478,7 +1527,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="n"/>
+      <c r="A26" s="9" t="n"/>
       <c r="B26" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -1516,7 +1565,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="n"/>
+      <c r="A27" s="9" t="n"/>
       <c r="B27" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -1554,7 +1603,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="n"/>
+      <c r="A28" s="9" t="n"/>
       <c r="B28" s="5" t="inlineStr">
         <is>
           <t>KGLL-KOC</t>
@@ -1592,7 +1641,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="n"/>
+      <c r="A29" s="9" t="n"/>
       <c r="B29" s="5" t="inlineStr">
         <is>
           <t>TC-BLKLT</t>
@@ -1630,7 +1679,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="n"/>
+      <c r="A30" s="9" t="n"/>
       <c r="B30" s="5" t="inlineStr">
         <is>
           <t>TC-TERMINL</t>
@@ -1668,7 +1717,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="n"/>
+      <c r="A31" s="9" t="n"/>
       <c r="B31" s="5" t="inlineStr">
         <is>
           <t>TC-MHECRAN</t>
@@ -1706,7 +1755,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="n"/>
+      <c r="A32" s="9" t="n"/>
       <c r="B32" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -1744,7 +1793,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="n"/>
+      <c r="A33" s="9" t="n"/>
       <c r="B33" s="5" t="inlineStr">
         <is>
           <t>TC-ES</t>
@@ -1782,7 +1831,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="n"/>
+      <c r="A34" s="10" t="n"/>
       <c r="B34" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -1862,7 +1911,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="n"/>
+      <c r="A36" s="9" t="n"/>
       <c r="B36" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -1900,7 +1949,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="n"/>
+      <c r="A37" s="9" t="n"/>
       <c r="B37" s="5" t="inlineStr">
         <is>
           <t>TC-US Govt</t>
@@ -1938,7 +1987,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="n"/>
+      <c r="A38" s="9" t="n"/>
       <c r="B38" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -1976,7 +2025,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="4" t="n"/>
+      <c r="A39" s="9" t="n"/>
       <c r="B39" s="5" t="inlineStr">
         <is>
           <t>FS-PV</t>
@@ -2014,7 +2063,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="4" t="n"/>
+      <c r="A40" s="9" t="n"/>
       <c r="B40" s="5" t="inlineStr">
         <is>
           <t>TC-KT</t>
@@ -2052,7 +2101,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="n"/>
+      <c r="A41" s="9" t="n"/>
       <c r="B41" s="5" t="inlineStr">
         <is>
           <t>TC-TERMINL</t>
@@ -2090,7 +2139,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="4" t="n"/>
+      <c r="A42" s="9" t="n"/>
       <c r="B42" s="5" t="inlineStr">
         <is>
           <t>TC-MHECRAN</t>
@@ -2128,7 +2177,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="4" t="n"/>
+      <c r="A43" s="9" t="n"/>
       <c r="B43" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -2166,7 +2215,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="4" t="n"/>
+      <c r="A44" s="9" t="n"/>
       <c r="B44" s="5" t="inlineStr">
         <is>
           <t>KGLL-KOC</t>
@@ -2204,7 +2253,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="4" t="n"/>
+      <c r="A45" s="9" t="n"/>
       <c r="B45" s="5" t="inlineStr">
         <is>
           <t>TC-ES</t>
@@ -2242,7 +2291,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="4" t="n"/>
+      <c r="A46" s="10" t="n"/>
       <c r="B46" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -2322,7 +2371,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="4" t="n"/>
+      <c r="A48" s="9" t="n"/>
       <c r="B48" s="5" t="inlineStr">
         <is>
           <t>TC-US Govt</t>
@@ -2360,7 +2409,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="4" t="n"/>
+      <c r="A49" s="9" t="n"/>
       <c r="B49" s="5" t="inlineStr">
         <is>
           <t>TS-MAB WS</t>
@@ -2398,7 +2447,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="4" t="n"/>
+      <c r="A50" s="9" t="n"/>
       <c r="B50" s="5" t="inlineStr">
         <is>
           <t>TC-TERMINL</t>
@@ -2436,7 +2485,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="4" t="n"/>
+      <c r="A51" s="9" t="n"/>
       <c r="B51" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -2474,7 +2523,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="4" t="n"/>
+      <c r="A52" s="9" t="n"/>
       <c r="B52" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -2512,7 +2561,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="4" t="n"/>
+      <c r="A53" s="9" t="n"/>
       <c r="B53" s="5" t="inlineStr">
         <is>
           <t>FS-PV</t>
@@ -2550,7 +2599,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="4" t="n"/>
+      <c r="A54" s="9" t="n"/>
       <c r="B54" s="5" t="inlineStr">
         <is>
           <t>TC-BLKLT</t>
@@ -2588,7 +2637,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="4" t="n"/>
+      <c r="A55" s="9" t="n"/>
       <c r="B55" s="5" t="inlineStr">
         <is>
           <t>TC-MHECRAN</t>
@@ -2626,7 +2675,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="4" t="n"/>
+      <c r="A56" s="9" t="n"/>
       <c r="B56" s="5" t="inlineStr">
         <is>
           <t>TC-ES</t>
@@ -2664,7 +2713,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="4" t="n"/>
+      <c r="A57" s="9" t="n"/>
       <c r="B57" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -2702,7 +2751,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="4" t="n"/>
+      <c r="A58" s="9" t="n"/>
       <c r="B58" s="5" t="inlineStr">
         <is>
           <t>KGLL-KOC</t>
@@ -2740,7 +2789,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="4" t="n"/>
+      <c r="A59" s="10" t="n"/>
       <c r="B59" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -2820,7 +2869,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="4" t="n"/>
+      <c r="A61" s="9" t="n"/>
       <c r="B61" s="5" t="inlineStr">
         <is>
           <t>TC-US Govt</t>
@@ -2858,7 +2907,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="4" t="n"/>
+      <c r="A62" s="9" t="n"/>
       <c r="B62" s="5" t="inlineStr">
         <is>
           <t>TC-KT</t>
@@ -2896,7 +2945,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="4" t="n"/>
+      <c r="A63" s="9" t="n"/>
       <c r="B63" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -2934,7 +2983,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="4" t="n"/>
+      <c r="A64" s="9" t="n"/>
       <c r="B64" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -2972,7 +3021,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="4" t="n"/>
+      <c r="A65" s="9" t="n"/>
       <c r="B65" s="5" t="inlineStr">
         <is>
           <t>FS-PV</t>
@@ -3010,7 +3059,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="4" t="n"/>
+      <c r="A66" s="9" t="n"/>
       <c r="B66" s="5" t="inlineStr">
         <is>
           <t>KGLL-KOC</t>
@@ -3048,7 +3097,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="4" t="n"/>
+      <c r="A67" s="9" t="n"/>
       <c r="B67" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -3086,7 +3135,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="4" t="n"/>
+      <c r="A68" s="9" t="n"/>
       <c r="B68" s="5" t="inlineStr">
         <is>
           <t>TC-TERMINL</t>
@@ -3124,7 +3173,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="4" t="n"/>
+      <c r="A69" s="9" t="n"/>
       <c r="B69" s="5" t="inlineStr">
         <is>
           <t>TC-ES</t>
@@ -3162,7 +3211,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="4" t="n"/>
+      <c r="A70" s="9" t="n"/>
       <c r="B70" s="5" t="inlineStr">
         <is>
           <t>TC-MHECRAN</t>
@@ -3200,7 +3249,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="4" t="n"/>
+      <c r="A71" s="9" t="n"/>
       <c r="B71" s="5" t="inlineStr">
         <is>
           <t>TS-MAB WS</t>
@@ -3238,7 +3287,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="4" t="n"/>
+      <c r="A72" s="10" t="n"/>
       <c r="B72" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -3318,7 +3367,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="4" t="n"/>
+      <c r="A74" s="9" t="n"/>
       <c r="B74" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -3356,7 +3405,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="4" t="n"/>
+      <c r="A75" s="9" t="n"/>
       <c r="B75" s="5" t="inlineStr">
         <is>
           <t>FS-PV</t>
@@ -3394,7 +3443,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="4" t="n"/>
+      <c r="A76" s="9" t="n"/>
       <c r="B76" s="5" t="inlineStr">
         <is>
           <t>TC-TERMINL</t>
@@ -3432,7 +3481,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="4" t="n"/>
+      <c r="A77" s="9" t="n"/>
       <c r="B77" s="5" t="inlineStr">
         <is>
           <t>TC-US Govt</t>
@@ -3470,7 +3519,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="4" t="n"/>
+      <c r="A78" s="9" t="n"/>
       <c r="B78" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -3508,7 +3557,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="4" t="n"/>
+      <c r="A79" s="9" t="n"/>
       <c r="B79" s="5" t="inlineStr">
         <is>
           <t>TC-OPEN</t>
@@ -3546,7 +3595,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="4" t="n"/>
+      <c r="A80" s="9" t="n"/>
       <c r="B80" s="5" t="inlineStr">
         <is>
           <t>TC-MHECRAN</t>
@@ -3584,7 +3633,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="4" t="n"/>
+      <c r="A81" s="9" t="n"/>
       <c r="B81" s="5" t="inlineStr">
         <is>
           <t>TS-MAB WS</t>
@@ -3622,7 +3671,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="4" t="n"/>
+      <c r="A82" s="9" t="n"/>
       <c r="B82" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -3660,7 +3709,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="4" t="n"/>
+      <c r="A83" s="10" t="n"/>
       <c r="B83" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -3740,7 +3789,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="4" t="n"/>
+      <c r="A85" s="9" t="n"/>
       <c r="B85" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -3778,7 +3827,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="4" t="n"/>
+      <c r="A86" s="9" t="n"/>
       <c r="B86" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -3816,7 +3865,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="4" t="n"/>
+      <c r="A87" s="9" t="n"/>
       <c r="B87" s="5" t="inlineStr">
         <is>
           <t>FS-PV</t>
@@ -3854,7 +3903,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="4" t="n"/>
+      <c r="A88" s="9" t="n"/>
       <c r="B88" s="5" t="inlineStr">
         <is>
           <t>TC-KT</t>
@@ -3892,7 +3941,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="4" t="n"/>
+      <c r="A89" s="9" t="n"/>
       <c r="B89" s="5" t="inlineStr">
         <is>
           <t>TC-BLKLT</t>
@@ -3930,7 +3979,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="4" t="n"/>
+      <c r="A90" s="9" t="n"/>
       <c r="B90" s="5" t="inlineStr">
         <is>
           <t>TC-MHECRAN</t>
@@ -3968,7 +4017,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="4" t="n"/>
+      <c r="A91" s="9" t="n"/>
       <c r="B91" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -4006,7 +4055,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="4" t="n"/>
+      <c r="A92" s="10" t="n"/>
       <c r="B92" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -4086,7 +4135,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="4" t="n"/>
+      <c r="A94" s="9" t="n"/>
       <c r="B94" s="5" t="inlineStr">
         <is>
           <t>TC-US Govt</t>
@@ -4124,7 +4173,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="4" t="n"/>
+      <c r="A95" s="9" t="n"/>
       <c r="B95" s="5" t="inlineStr">
         <is>
           <t>TC-ES</t>
@@ -4162,7 +4211,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="4" t="n"/>
+      <c r="A96" s="9" t="n"/>
       <c r="B96" s="5" t="inlineStr">
         <is>
           <t>PTS-SPRENT</t>
@@ -4200,7 +4249,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="4" t="n"/>
+      <c r="A97" s="9" t="n"/>
       <c r="B97" s="5" t="inlineStr">
         <is>
           <t>TC-KT</t>
@@ -4238,7 +4287,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="4" t="n"/>
+      <c r="A98" s="9" t="n"/>
       <c r="B98" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -4276,7 +4325,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="4" t="n"/>
+      <c r="A99" s="9" t="n"/>
       <c r="B99" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -4314,7 +4363,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="4" t="n"/>
+      <c r="A100" s="9" t="n"/>
       <c r="B100" s="5" t="inlineStr">
         <is>
           <t>TC-TERMINL</t>
@@ -4352,7 +4401,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="4" t="n"/>
+      <c r="A101" s="9" t="n"/>
       <c r="B101" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -4390,7 +4439,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="4" t="n"/>
+      <c r="A102" s="9" t="n"/>
       <c r="B102" s="5" t="inlineStr">
         <is>
           <t>TC-BLKLT</t>
@@ -4428,7 +4477,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="4" t="n"/>
+      <c r="A103" s="9" t="n"/>
       <c r="B103" s="5" t="inlineStr">
         <is>
           <t>TC-MHECRAN</t>
@@ -4466,7 +4515,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="4" t="n"/>
+      <c r="A104" s="10" t="n"/>
       <c r="B104" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -4546,7 +4595,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="4" t="n"/>
+      <c r="A106" s="9" t="n"/>
       <c r="B106" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -4584,7 +4633,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="4" t="n"/>
+      <c r="A107" s="9" t="n"/>
       <c r="B107" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -4622,7 +4671,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="4" t="n"/>
+      <c r="A108" s="9" t="n"/>
       <c r="B108" s="5" t="inlineStr">
         <is>
           <t>TC-MHECRAN</t>
@@ -4660,7 +4709,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="4" t="n"/>
+      <c r="A109" s="9" t="n"/>
       <c r="B109" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -4698,7 +4747,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="4" t="n"/>
+      <c r="A110" s="9" t="n"/>
       <c r="B110" s="5" t="inlineStr">
         <is>
           <t>FS-PV</t>
@@ -4736,7 +4785,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="4" t="n"/>
+      <c r="A111" s="9" t="n"/>
       <c r="B111" s="5" t="inlineStr">
         <is>
           <t>TC-KT</t>
@@ -4774,7 +4823,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="4" t="n"/>
+      <c r="A112" s="9" t="n"/>
       <c r="B112" s="5" t="inlineStr">
         <is>
           <t>TC-ES</t>
@@ -4812,7 +4861,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="4" t="n"/>
+      <c r="A113" s="10" t="n"/>
       <c r="B113" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -4892,7 +4941,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="4" t="n"/>
+      <c r="A115" s="9" t="n"/>
       <c r="B115" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -4930,7 +4979,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="4" t="n"/>
+      <c r="A116" s="9" t="n"/>
       <c r="B116" s="5" t="inlineStr">
         <is>
           <t>FS-PV</t>
@@ -4968,7 +5017,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="4" t="n"/>
+      <c r="A117" s="9" t="n"/>
       <c r="B117" s="5" t="inlineStr">
         <is>
           <t>TC-KT</t>
@@ -5006,7 +5055,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="4" t="n"/>
+      <c r="A118" s="9" t="n"/>
       <c r="B118" s="5" t="inlineStr">
         <is>
           <t>TC-TERMINL</t>
@@ -5044,7 +5093,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="4" t="n"/>
+      <c r="A119" s="9" t="n"/>
       <c r="B119" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -5082,7 +5131,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="4" t="n"/>
+      <c r="A120" s="9" t="n"/>
       <c r="B120" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -5120,7 +5169,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="4" t="n"/>
+      <c r="A121" s="9" t="n"/>
       <c r="B121" s="5" t="inlineStr">
         <is>
           <t>TC-MHECRAN</t>
@@ -5158,7 +5207,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="4" t="n"/>
+      <c r="A122" s="9" t="n"/>
       <c r="B122" s="5" t="inlineStr">
         <is>
           <t>TS-MAB WS</t>
@@ -5196,7 +5245,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="4" t="n"/>
+      <c r="A123" s="10" t="n"/>
       <c r="B123" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -5276,7 +5325,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="4" t="n"/>
+      <c r="A125" s="9" t="n"/>
       <c r="B125" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -5314,7 +5363,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="4" t="n"/>
+      <c r="A126" s="9" t="n"/>
       <c r="B126" s="5" t="inlineStr">
         <is>
           <t>FS-PV</t>
@@ -5352,7 +5401,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="4" t="n"/>
+      <c r="A127" s="9" t="n"/>
       <c r="B127" s="5" t="inlineStr">
         <is>
           <t>TC-TERMINL</t>
@@ -5390,7 +5439,7 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="4" t="n"/>
+      <c r="A128" s="9" t="n"/>
       <c r="B128" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -5428,7 +5477,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="4" t="n"/>
+      <c r="A129" s="9" t="n"/>
       <c r="B129" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -5466,7 +5515,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="4" t="n"/>
+      <c r="A130" s="9" t="n"/>
       <c r="B130" s="5" t="inlineStr">
         <is>
           <t>TC-KT</t>
@@ -5504,7 +5553,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="4" t="n"/>
+      <c r="A131" s="9" t="n"/>
       <c r="B131" s="5" t="inlineStr">
         <is>
           <t>TC-BLKLT</t>
@@ -5542,7 +5591,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="4" t="n"/>
+      <c r="A132" s="9" t="n"/>
       <c r="B132" s="5" t="inlineStr">
         <is>
           <t>TC-ES</t>
@@ -5580,7 +5629,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="4" t="n"/>
+      <c r="A133" s="9" t="n"/>
       <c r="B133" s="5" t="inlineStr">
         <is>
           <t>TC-MHECRAN</t>
@@ -5618,7 +5667,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="4" t="n"/>
+      <c r="A134" s="10" t="n"/>
       <c r="B134" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -5698,7 +5747,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="4" t="n"/>
+      <c r="A136" s="9" t="n"/>
       <c r="B136" s="5" t="inlineStr">
         <is>
           <t>TC-BLKLT</t>
@@ -5736,7 +5785,7 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="4" t="n"/>
+      <c r="A137" s="9" t="n"/>
       <c r="B137" s="5" t="inlineStr">
         <is>
           <t>FS-PV</t>
@@ -5774,7 +5823,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="4" t="n"/>
+      <c r="A138" s="9" t="n"/>
       <c r="B138" s="5" t="inlineStr">
         <is>
           <t>TC-KT</t>
@@ -5812,7 +5861,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="4" t="n"/>
+      <c r="A139" s="9" t="n"/>
       <c r="B139" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -5850,7 +5899,7 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="4" t="n"/>
+      <c r="A140" s="9" t="n"/>
       <c r="B140" s="5" t="inlineStr">
         <is>
           <t>TC-TERMINL</t>
@@ -5888,7 +5937,7 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="4" t="n"/>
+      <c r="A141" s="9" t="n"/>
       <c r="B141" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -5926,7 +5975,7 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="4" t="n"/>
+      <c r="A142" s="9" t="n"/>
       <c r="B142" s="5" t="inlineStr">
         <is>
           <t>TC-MHECRAN</t>
@@ -5964,7 +6013,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="4" t="n"/>
+      <c r="A143" s="9" t="n"/>
       <c r="B143" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -6002,7 +6051,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="4" t="n"/>
+      <c r="A144" s="10" t="n"/>
       <c r="B144" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -6082,7 +6131,7 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="4" t="n"/>
+      <c r="A146" s="9" t="n"/>
       <c r="B146" s="5" t="inlineStr">
         <is>
           <t>TC-KT</t>
@@ -6120,7 +6169,7 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="4" t="n"/>
+      <c r="A147" s="9" t="n"/>
       <c r="B147" s="5" t="inlineStr">
         <is>
           <t>TC-US Govt</t>
@@ -6158,7 +6207,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="4" t="n"/>
+      <c r="A148" s="9" t="n"/>
       <c r="B148" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -6196,7 +6245,7 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="4" t="n"/>
+      <c r="A149" s="9" t="n"/>
       <c r="B149" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -6234,7 +6283,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="4" t="n"/>
+      <c r="A150" s="9" t="n"/>
       <c r="B150" s="5" t="inlineStr">
         <is>
           <t>FS-PV</t>
@@ -6272,7 +6321,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="4" t="n"/>
+      <c r="A151" s="9" t="n"/>
       <c r="B151" s="5" t="inlineStr">
         <is>
           <t>TC-TERMINL</t>
@@ -6310,7 +6359,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="4" t="n"/>
+      <c r="A152" s="9" t="n"/>
       <c r="B152" s="5" t="inlineStr">
         <is>
           <t>TC-BLKLT</t>
@@ -6348,7 +6397,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="4" t="n"/>
+      <c r="A153" s="10" t="n"/>
       <c r="B153" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -6428,7 +6477,7 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="4" t="n"/>
+      <c r="A155" s="9" t="n"/>
       <c r="B155" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -6466,7 +6515,7 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="4" t="n"/>
+      <c r="A156" s="9" t="n"/>
       <c r="B156" s="5" t="inlineStr">
         <is>
           <t>TC-US Govt</t>
@@ -6504,7 +6553,7 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="4" t="n"/>
+      <c r="A157" s="9" t="n"/>
       <c r="B157" s="5" t="inlineStr">
         <is>
           <t>TC-KT</t>
@@ -6542,7 +6591,7 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="4" t="n"/>
+      <c r="A158" s="9" t="n"/>
       <c r="B158" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -6580,7 +6629,7 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="4" t="n"/>
+      <c r="A159" s="9" t="n"/>
       <c r="B159" s="5" t="inlineStr">
         <is>
           <t>FS-PV</t>
@@ -6618,7 +6667,7 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="4" t="n"/>
+      <c r="A160" s="9" t="n"/>
       <c r="B160" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -6656,7 +6705,7 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="4" t="n"/>
+      <c r="A161" s="10" t="n"/>
       <c r="B161" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -6736,7 +6785,7 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="4" t="n"/>
+      <c r="A163" s="9" t="n"/>
       <c r="B163" s="5" t="inlineStr">
         <is>
           <t>FS-PV</t>
@@ -6774,7 +6823,7 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="4" t="n"/>
+      <c r="A164" s="9" t="n"/>
       <c r="B164" s="5" t="inlineStr">
         <is>
           <t>TC-TERMINL</t>
@@ -6812,7 +6861,7 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="4" t="n"/>
+      <c r="A165" s="9" t="n"/>
       <c r="B165" s="5" t="inlineStr">
         <is>
           <t>TC-KT</t>
@@ -6850,7 +6899,7 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" s="4" t="n"/>
+      <c r="A166" s="9" t="n"/>
       <c r="B166" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -6888,7 +6937,7 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="4" t="n"/>
+      <c r="A167" s="9" t="n"/>
       <c r="B167" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -6926,7 +6975,7 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="4" t="n"/>
+      <c r="A168" s="9" t="n"/>
       <c r="B168" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -6964,7 +7013,7 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="4" t="n"/>
+      <c r="A169" s="9" t="n"/>
       <c r="B169" s="5" t="inlineStr">
         <is>
           <t>TC-ES</t>
@@ -7002,7 +7051,7 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="4" t="n"/>
+      <c r="A170" s="9" t="n"/>
       <c r="B170" s="5" t="inlineStr">
         <is>
           <t>TC-BLKLT</t>
@@ -7040,7 +7089,7 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="4" t="n"/>
+      <c r="A171" s="10" t="n"/>
       <c r="B171" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -7120,7 +7169,7 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="4" t="n"/>
+      <c r="A173" s="9" t="n"/>
       <c r="B173" s="5" t="inlineStr">
         <is>
           <t>FS-PV</t>
@@ -7158,7 +7207,7 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="4" t="n"/>
+      <c r="A174" s="9" t="n"/>
       <c r="B174" s="5" t="inlineStr">
         <is>
           <t>KGLL-KOC</t>
@@ -7196,7 +7245,7 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" s="4" t="n"/>
+      <c r="A175" s="9" t="n"/>
       <c r="B175" s="5" t="inlineStr">
         <is>
           <t>TC-OVRLAND</t>
@@ -7234,7 +7283,7 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="4" t="n"/>
+      <c r="A176" s="9" t="n"/>
       <c r="B176" s="5" t="inlineStr">
         <is>
           <t>AL-ASTPOOL</t>
@@ -7272,7 +7321,7 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="4" t="n"/>
+      <c r="A177" s="9" t="n"/>
       <c r="B177" s="5" t="inlineStr">
         <is>
           <t>TC-KT</t>
@@ -7310,7 +7359,7 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="4" t="n"/>
+      <c r="A178" s="9" t="n"/>
       <c r="B178" s="5" t="inlineStr">
         <is>
           <t>TC-KNPCFT</t>
@@ -7348,7 +7397,7 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" s="4" t="n"/>
+      <c r="A179" s="9" t="n"/>
       <c r="B179" s="5" t="inlineStr">
         <is>
           <t>TC-ES</t>
@@ -7386,7 +7435,7 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="4" t="n"/>
+      <c r="A180" s="10" t="n"/>
       <c r="B180" s="6" t="inlineStr">
         <is>
           <t>Total</t>
@@ -7423,15 +7472,6 @@
         <v>439.5300000000001</v>
       </c>
     </row>
-    <row r="181" hidden="1"/>
-    <row r="182" hidden="1"/>
-    <row r="183" hidden="1"/>
-    <row r="184" hidden="1"/>
-    <row r="185" hidden="1"/>
-    <row r="186" hidden="1"/>
-    <row r="187" hidden="1"/>
-    <row r="188" hidden="1"/>
-    <row r="189" hidden="1"/>
   </sheetData>
   <mergeCells count="18">
     <mergeCell ref="A154:A161"/>
@@ -7439,19 +7479,699 @@
     <mergeCell ref="A162:A171"/>
     <mergeCell ref="A114:A123"/>
     <mergeCell ref="A145:A153"/>
-    <mergeCell ref="A84:A92"/>
+    <mergeCell ref="A105:A113"/>
     <mergeCell ref="A93:A104"/>
     <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A105:A113"/>
+    <mergeCell ref="A135:A144"/>
     <mergeCell ref="A73:A83"/>
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="A23:A34"/>
     <mergeCell ref="A47:A59"/>
-    <mergeCell ref="A135:A144"/>
     <mergeCell ref="A172:A180"/>
     <mergeCell ref="A124:A134"/>
     <mergeCell ref="A60:A72"/>
     <mergeCell ref="A35:A46"/>
+    <mergeCell ref="A84:A92"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="9" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="18" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Work Order Status Report</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Project</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Total WO</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>Cancelled</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>On Hold</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>Released</t>
+        </is>
+      </c>
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>Vehicle Released</t>
+        </is>
+      </c>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>Workshop Completed</t>
+        </is>
+      </c>
+      <c r="K2" s="3" t="inlineStr">
+        <is>
+          <t>Workshop Checked In</t>
+        </is>
+      </c>
+      <c r="L2" s="3" t="inlineStr">
+        <is>
+          <t>Material cost</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>2025-08</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>PTS-SPRENT</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n"/>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>TC-KT</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>102</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <v>73</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>887.4299999999998</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n"/>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>TC-US Govt</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>500</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>56</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>82</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <v>302</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <v>5868.800000000007</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n"/>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>TC-OVRLAND</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>63</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <v>2090.8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n"/>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>FS-PV</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>172</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <v>109</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <v>2006.049999999999</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n"/>
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>TC-KNPCFT</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>68</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="J8" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="5" t="n">
+        <v>962.3000000000001</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n"/>
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>TC-ES</t>
+        </is>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J9" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="5" t="n">
+        <v>117.66</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n"/>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>TS-MAB WS</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5" t="n">
+        <v>25.82</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n"/>
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>AL-ASTPOOL</t>
+        </is>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>162</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="J11" s="5" t="n">
+        <v>121</v>
+      </c>
+      <c r="K11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n"/>
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>TC-BLKLT</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K12" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="L12" s="5" t="n">
+        <v>203.71</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>TC-TERMINL</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J13" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="K13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="5" t="n">
+        <v>132.16</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>KGLL-KOC</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J14" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K14" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="L14" s="5" t="n">
+        <v>21.22</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>TC-MHECRAN</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="K15" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="L15" s="5" t="n">
+        <v>321.4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n"/>
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t>TC-OPEN</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n"/>
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>1147</v>
+      </c>
+      <c r="D17" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F17" s="6" t="n">
+        <v>98</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="H17" s="6" t="n">
+        <v>36</v>
+      </c>
+      <c r="I17" s="6" t="n">
+        <v>189</v>
+      </c>
+      <c r="J17" s="6" t="n">
+        <v>715</v>
+      </c>
+      <c r="K17" s="6" t="n">
+        <v>74</v>
+      </c>
+      <c r="L17" s="6" t="n">
+        <v>12639.60000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A17"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>